<commit_message>
Scraper put into function
</commit_message>
<xml_diff>
--- a/out/artifacts/Team_match_verify_jar/TeamMatchVerify.xlsx
+++ b/out/artifacts/Team_match_verify_jar/TeamMatchVerify.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\OneDrive\Skrivebord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Team-match-verify\out\artifacts\Team_match_verify_jar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A5E52E-E526-4E0E-859A-2389B9E46B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EE6A33-EBE5-42F0-BE1E-86A39AAC7523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BEABDDE-1E11-4A13-BD8F-012D9F57800C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1BEABDDE-1E11-4A13-BD8F-012D9F57800C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -595,43 +595,43 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6C28B2-4096-4F62-8A60-1FF17FE97E75}">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1073,22 +1073,22 @@
       </c>
     </row>
     <row r="2" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="15">
         <f>INDEX(RankList[],MATCH(C2,RankList[Name],0),6)</f>
         <v>3190</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="34">
         <f>E2+E3</f>
         <v>5916</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="32">
         <f>(F2+100)-F4</f>
         <v>171</v>
       </c>
@@ -1096,7 +1096,7 @@
         <f>INDEX(RankList[],MATCH(C2,RankList[Name],0),2)</f>
         <v>m</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="29">
         <f>IF(H2=H3,1,0)</f>
         <v>0</v>
       </c>
@@ -1106,49 +1106,49 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="15">
         <f>INDEX(RankList[],MATCH(C3,RankList[Name],0),6)</f>
         <v>2726</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C3,RankList[Name],0),2)</f>
         <v>w</v>
       </c>
-      <c r="I3" s="35"/>
+      <c r="I3" s="29"/>
       <c r="J3" s="26">
         <f t="shared" ref="J3:J21" si="0">COUNTIF($C$2:$C$21,C3)</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="15">
         <f>INDEX(RankList[],MATCH(C4,RankList[Name],0),6)</f>
         <v>3200</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="34">
         <f>E4+E5</f>
         <v>5845</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C4,RankList[Name],0),2)</f>
         <v>m</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="29">
         <f>IF(H4=H5,1,0)</f>
         <v>0</v>
       </c>
@@ -1158,22 +1158,22 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="15">
         <f>INDEX(RankList[],MATCH(C5,RankList[Name],0),6)</f>
         <v>2645</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="32"/>
       <c r="H5" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C5,RankList[Name],0),2)</f>
         <v>w</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="26">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1372,22 +1372,22 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="38" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="15">
         <f>INDEX(RankList[],MATCH(C12,RankList[Name],0),5)</f>
         <v>2942</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="34">
         <f t="shared" ref="F12" si="4">E12+E13</f>
         <v>5305</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="32">
         <f>F12-F14</f>
         <v>51</v>
       </c>
@@ -1405,17 +1405,17 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="15">
         <f>INDEX(RankList[],MATCH(C13,RankList[Name],0),5)</f>
         <v>2363</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C13,RankList[Name],0),2)</f>
         <v>w</v>
@@ -1430,22 +1430,22 @@
       </c>
     </row>
     <row r="14" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="15">
         <f>INDEX(RankList[],MATCH(C14,RankList[Name],0),5)</f>
         <v>2656</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="34">
         <f t="shared" ref="F14" si="6">E14+E15</f>
         <v>5254</v>
       </c>
-      <c r="G14" s="34"/>
+      <c r="G14" s="32"/>
       <c r="H14" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C14,RankList[Name],0),2)</f>
         <v>w</v>
@@ -1460,17 +1460,17 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="31"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="15">
         <f>INDEX(RankList[],MATCH(C15,RankList[Name],0),5)</f>
         <v>2598</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C15,RankList[Name],0),2)</f>
         <v>w</v>
@@ -1485,22 +1485,22 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="15">
         <f>INDEX(RankList[],MATCH(C16,RankList[Name],0),5)</f>
         <v>3363</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="34">
         <f t="shared" ref="F16" si="7">E16+E17</f>
         <v>6686</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="32">
         <f>F16-F18</f>
         <v>-66</v>
       </c>
@@ -1518,17 +1518,17 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="37"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="15">
         <f>INDEX(RankList[],MATCH(C17,RankList[Name],0),5)</f>
         <v>3323</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C17,RankList[Name],0),2)</f>
         <v>m</v>
@@ -1543,22 +1543,22 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="36"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="15">
         <f>INDEX(RankList[],MATCH(C18,RankList[Name],0),5)</f>
         <v>3326</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="34">
         <f t="shared" ref="F18" si="9">E18+E19</f>
         <v>6752</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="32">
         <f>F18-F20</f>
         <v>151</v>
       </c>
@@ -1576,17 +1576,17 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="33"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="37"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="15">
         <f>INDEX(RankList[],MATCH(C19,RankList[Name],0),5)</f>
         <v>3426</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="32"/>
       <c r="H19" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C19,RankList[Name],0),2)</f>
         <v>m</v>
@@ -1601,22 +1601,22 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="36" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="36"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="15">
         <f>INDEX(RankList[],MATCH(C20,RankList[Name],0),5)</f>
         <v>3241</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="34">
         <f t="shared" ref="F20" si="10">E20+E21</f>
         <v>6601</v>
       </c>
-      <c r="G20" s="34"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="20" t="str">
         <f>INDEX(RankList[],MATCH(C20,RankList[Name],0),2)</f>
         <v>m</v>
@@ -1631,17 +1631,17 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="37"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="18">
         <f>INDEX(RankList[],MATCH(C21,RankList[Name],0),5)</f>
         <v>3360</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="38"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="33"/>
       <c r="H21" s="21" t="str">
         <f>INDEX(RankList[],MATCH(C21,RankList[Name],0),2)</f>
         <v>m</v>
@@ -1657,6 +1657,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F14:F15"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="D16:D17"/>
@@ -1673,20 +1687,6 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <conditionalFormatting sqref="F2 F4 F6:F12 F14 F16 F18">
     <cfRule type="expression" dxfId="6" priority="7">
@@ -1733,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8259F9-40D9-48AB-9DC6-084747F0F304}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E25:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>